<commit_message>
ajustes menu e cores
</commit_message>
<xml_diff>
--- a/planilhas/Contabilidade Condominio.xlsx
+++ b/planilhas/Contabilidade Condominio.xlsx
@@ -5358,15 +5358,33 @@
       <c r="A14" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="96"/>
-      <c r="C14" s="96"/>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="96"/>
+      <c r="B14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="C14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="D14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="E14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="96">
+        <v>0.0</v>
+      </c>
       <c r="K14" s="96">
         <v>0.0</v>
       </c>

</xml_diff>